<commit_message>
feat : adicionando o firebase
</commit_message>
<xml_diff>
--- a/nome-servidores.xlsx
+++ b/nome-servidores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\70352867213\projetos-sejusc\SEJUSC\sistema_frequenciaRH_site\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\70352867213\projetos_sejusc\SISTEMA-DE-FREQUENCIA-WEB-BACK-END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E88C9F-AE78-4C21-9375-4533A609023B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5786A02E-5AFA-4E42-B73D-3687B835C2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="1485" windowWidth="22080" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -2126,8 +2126,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm:ss\ \t\t"/>
+    <numFmt numFmtId="169" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -2191,11 +2192,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="19" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2504,7 +2505,7 @@
   <dimension ref="A1:L290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2570,10 +2571,10 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="G2" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H2" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2593,10 +2594,10 @@
       <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="G3" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H3" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2616,10 +2617,10 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G4" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H4" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2639,10 +2640,10 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G5" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H5" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2662,10 +2663,10 @@
       <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H6" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2685,13 +2686,13 @@
       <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I7" s="4"/>
+      <c r="G7" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2709,10 +2710,10 @@
       <c r="F8" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G8" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H8" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2732,13 +2733,13 @@
       <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="G9" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H9" s="5">
         <v>1.5839814814814814</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2756,10 +2757,10 @@
       <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="G10" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H10" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2779,10 +2780,10 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="G11" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H11" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2802,10 +2803,10 @@
       <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="G12" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H12" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2825,16 +2826,16 @@
       <c r="F13" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H13" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I13" s="5">
+      <c r="G13" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I13" s="4">
         <v>45719</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -2854,10 +2855,10 @@
       <c r="F14" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="G14" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H14" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2877,10 +2878,10 @@
       <c r="F15" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="G15" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H15" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -2900,10 +2901,10 @@
       <c r="F16" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H16" s="3">
+      <c r="G16" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H16" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2923,10 +2924,10 @@
       <c r="F17" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="G17" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H17" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2946,10 +2947,10 @@
       <c r="F18" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H18" s="3">
+      <c r="G18" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H18" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2969,10 +2970,10 @@
       <c r="F19" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H19" s="3">
+      <c r="G19" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H19" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -2992,10 +2993,10 @@
       <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H20" s="3">
+      <c r="G20" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H20" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3015,16 +3016,16 @@
       <c r="F21" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H21" s="3">
+      <c r="G21" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H21" s="5">
         <v>1.5839814814814814</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="4">
         <v>45719</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -3044,10 +3045,10 @@
       <c r="F22" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="G22" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H22" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3067,10 +3068,10 @@
       <c r="F23" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H23" s="3">
+      <c r="G23" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H23" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3090,10 +3091,10 @@
       <c r="F24" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H24" s="3">
+      <c r="G24" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H24" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3113,10 +3114,10 @@
       <c r="F25" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H25" s="3">
+      <c r="G25" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H25" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3136,10 +3137,10 @@
       <c r="F26" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="G26" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H26" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3159,10 +3160,10 @@
       <c r="F27" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H27" s="3">
+      <c r="G27" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H27" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3182,10 +3183,10 @@
       <c r="F28" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H28" s="3">
+      <c r="G28" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H28" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3205,10 +3206,10 @@
       <c r="F29" t="s">
         <v>504</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="5">
         <v>1.7923148148148149</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="5">
         <v>1.2923148148148149</v>
       </c>
     </row>
@@ -3228,16 +3229,16 @@
       <c r="F30" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H30" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I30" s="5">
+      <c r="G30" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I30" s="4">
         <v>45722</v>
       </c>
-      <c r="J30" s="5">
+      <c r="J30" s="4">
         <v>45751</v>
       </c>
     </row>
@@ -3257,16 +3258,16 @@
       <c r="F31" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H31" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I31" s="5">
+      <c r="G31" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I31" s="4">
         <v>45719</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J31" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -3286,10 +3287,10 @@
       <c r="F32" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H32" s="3">
+      <c r="G32" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H32" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3309,10 +3310,10 @@
       <c r="F33" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H33" s="3">
+      <c r="G33" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H33" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3332,10 +3333,10 @@
       <c r="F34" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H34" s="3">
+      <c r="G34" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H34" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3355,10 +3356,10 @@
       <c r="F35" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H35" s="3">
+      <c r="G35" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H35" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3378,10 +3379,10 @@
       <c r="F36" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H36" s="3">
+      <c r="G36" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H36" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3401,10 +3402,10 @@
       <c r="F37" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H37" s="3">
+      <c r="G37" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H37" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3424,10 +3425,10 @@
       <c r="F38" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H38" s="3">
+      <c r="G38" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H38" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3447,16 +3448,16 @@
       <c r="F39" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H39" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I39" s="5">
+      <c r="G39" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I39" s="4">
         <v>45719</v>
       </c>
-      <c r="J39" s="5">
+      <c r="J39" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -3476,10 +3477,10 @@
       <c r="F40" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H40" s="3">
+      <c r="G40" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H40" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3499,10 +3500,10 @@
       <c r="F41" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H41" s="3">
+      <c r="G41" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H41" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3522,10 +3523,10 @@
       <c r="F42" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H42" s="3">
+      <c r="G42" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H42" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3545,10 +3546,10 @@
       <c r="F43" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H43" s="3">
+      <c r="G43" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H43" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3568,10 +3569,10 @@
       <c r="F44" t="s">
         <v>8</v>
       </c>
-      <c r="G44" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H44" s="3">
+      <c r="G44" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H44" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3591,10 +3592,10 @@
       <c r="F45" t="s">
         <v>8</v>
       </c>
-      <c r="G45" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H45" s="3">
+      <c r="G45" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H45" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3614,10 +3615,10 @@
       <c r="F46" t="s">
         <v>8</v>
       </c>
-      <c r="G46" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H46" s="3">
+      <c r="G46" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H46" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3637,10 +3638,10 @@
       <c r="F47" t="s">
         <v>185</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="5">
         <v>1.4589814814814814</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3660,10 +3661,10 @@
       <c r="F48" t="s">
         <v>26</v>
       </c>
-      <c r="G48" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H48" s="3">
+      <c r="G48" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H48" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -3683,10 +3684,10 @@
       <c r="F49" t="s">
         <v>427</v>
       </c>
-      <c r="G49" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H49" s="3">
+      <c r="G49" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H49" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3706,10 +3707,10 @@
       <c r="F50" t="s">
         <v>8</v>
       </c>
-      <c r="G50" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H50" s="3">
+      <c r="G50" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H50" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3729,10 +3730,10 @@
       <c r="F51" t="s">
         <v>8</v>
       </c>
-      <c r="G51" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H51" s="3">
+      <c r="G51" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H51" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3752,10 +3753,10 @@
       <c r="F52" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H52" s="3">
+      <c r="G52" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H52" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3775,10 +3776,10 @@
       <c r="F53" t="s">
         <v>8</v>
       </c>
-      <c r="G53" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H53" s="3">
+      <c r="G53" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H53" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3798,10 +3799,10 @@
       <c r="F54" t="s">
         <v>8</v>
       </c>
-      <c r="G54" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H54" s="3">
+      <c r="G54" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H54" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3821,10 +3822,10 @@
       <c r="F55" t="s">
         <v>8</v>
       </c>
-      <c r="G55" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H55" s="3">
+      <c r="G55" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H55" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3844,10 +3845,10 @@
       <c r="F56" t="s">
         <v>8</v>
       </c>
-      <c r="G56" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H56" s="3">
+      <c r="G56" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H56" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3867,10 +3868,10 @@
       <c r="F57" t="s">
         <v>8</v>
       </c>
-      <c r="G57" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H57" s="3">
+      <c r="G57" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H57" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3890,10 +3891,10 @@
       <c r="F58" t="s">
         <v>8</v>
       </c>
-      <c r="G58" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H58" s="3">
+      <c r="G58" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H58" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3913,10 +3914,10 @@
       <c r="F59" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H59" s="3">
+      <c r="G59" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H59" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3936,10 +3937,10 @@
       <c r="F60" t="s">
         <v>8</v>
       </c>
-      <c r="G60" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H60" s="3">
+      <c r="G60" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H60" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3959,10 +3960,10 @@
       <c r="F61" t="s">
         <v>8</v>
       </c>
-      <c r="G61" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H61" s="3">
+      <c r="G61" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H61" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -3982,10 +3983,10 @@
       <c r="F62" t="s">
         <v>26</v>
       </c>
-      <c r="G62" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H62" s="3">
+      <c r="G62" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H62" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -4005,10 +4006,10 @@
       <c r="F63" t="s">
         <v>8</v>
       </c>
-      <c r="G63" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H63" s="3">
+      <c r="G63" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H63" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4028,10 +4029,10 @@
       <c r="F64" t="s">
         <v>8</v>
       </c>
-      <c r="G64" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H64" s="3">
+      <c r="G64" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H64" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4051,10 +4052,10 @@
       <c r="F65" t="s">
         <v>8</v>
       </c>
-      <c r="G65" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H65" s="3">
+      <c r="G65" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H65" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4074,10 +4075,10 @@
       <c r="F66" t="s">
         <v>8</v>
       </c>
-      <c r="G66" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H66" s="3">
+      <c r="G66" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H66" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4097,10 +4098,10 @@
       <c r="F67" t="s">
         <v>8</v>
       </c>
-      <c r="G67" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H67" s="3">
+      <c r="G67" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H67" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4120,16 +4121,16 @@
       <c r="F68" t="s">
         <v>8</v>
       </c>
-      <c r="G68" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H68" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I68" s="5">
+      <c r="G68" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H68" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I68" s="4">
         <v>45719</v>
       </c>
-      <c r="J68" s="5">
+      <c r="J68" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -4149,10 +4150,10 @@
       <c r="F69" t="s">
         <v>8</v>
       </c>
-      <c r="G69" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H69" s="3">
+      <c r="G69" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H69" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4172,10 +4173,10 @@
       <c r="F70" t="s">
         <v>8</v>
       </c>
-      <c r="G70" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H70" s="3">
+      <c r="G70" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H70" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4195,10 +4196,10 @@
       <c r="F71" t="s">
         <v>26</v>
       </c>
-      <c r="G71" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H71" s="3">
+      <c r="G71" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H71" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -4218,10 +4219,10 @@
       <c r="F72" t="s">
         <v>8</v>
       </c>
-      <c r="G72" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H72" s="3">
+      <c r="G72" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H72" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4241,10 +4242,10 @@
       <c r="F73" t="s">
         <v>8</v>
       </c>
-      <c r="G73" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H73" s="3">
+      <c r="G73" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H73" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4264,10 +4265,10 @@
       <c r="F74" t="s">
         <v>8</v>
       </c>
-      <c r="G74" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H74" s="3">
+      <c r="G74" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H74" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4287,10 +4288,10 @@
       <c r="F75" t="s">
         <v>427</v>
       </c>
-      <c r="G75" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H75" s="3">
+      <c r="G75" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H75" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4310,10 +4311,10 @@
       <c r="F76" t="s">
         <v>8</v>
       </c>
-      <c r="G76" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H76" s="3">
+      <c r="G76" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H76" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4333,10 +4334,10 @@
       <c r="F77" t="s">
         <v>8</v>
       </c>
-      <c r="G77" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H77" s="3">
+      <c r="G77" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H77" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4356,10 +4357,10 @@
       <c r="F78" t="s">
         <v>8</v>
       </c>
-      <c r="G78" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H78" s="3">
+      <c r="G78" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H78" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4379,10 +4380,10 @@
       <c r="F79" t="s">
         <v>8</v>
       </c>
-      <c r="G79" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H79" s="3">
+      <c r="G79" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H79" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4402,10 +4403,10 @@
       <c r="F80" t="s">
         <v>8</v>
       </c>
-      <c r="G80" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H80" s="3">
+      <c r="G80" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H80" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4425,10 +4426,10 @@
       <c r="F81" t="s">
         <v>8</v>
       </c>
-      <c r="G81" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H81" s="3">
+      <c r="G81" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H81" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4448,10 +4449,10 @@
       <c r="F82" t="s">
         <v>8</v>
       </c>
-      <c r="G82" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H82" s="3">
+      <c r="G82" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H82" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4471,16 +4472,16 @@
       <c r="F83" t="s">
         <v>8</v>
       </c>
-      <c r="G83" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H83" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I83" s="5">
+      <c r="G83" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H83" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I83" s="4">
         <v>45719</v>
       </c>
-      <c r="J83" s="5">
+      <c r="J83" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -4500,10 +4501,10 @@
       <c r="F84" t="s">
         <v>8</v>
       </c>
-      <c r="G84" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H84" s="3">
+      <c r="G84" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H84" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4523,10 +4524,10 @@
       <c r="F85" t="s">
         <v>8</v>
       </c>
-      <c r="G85" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H85" s="3">
+      <c r="G85" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H85" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4546,10 +4547,10 @@
       <c r="F86" t="s">
         <v>8</v>
       </c>
-      <c r="G86" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H86" s="3">
+      <c r="G86" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H86" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4569,10 +4570,10 @@
       <c r="F87" t="s">
         <v>26</v>
       </c>
-      <c r="G87" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H87" s="3">
+      <c r="G87" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H87" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -4592,10 +4593,10 @@
       <c r="F88" t="s">
         <v>8</v>
       </c>
-      <c r="G88" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H88" s="3">
+      <c r="G88" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H88" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4615,10 +4616,10 @@
       <c r="F89" t="s">
         <v>504</v>
       </c>
-      <c r="G89" s="3">
+      <c r="G89" s="5">
         <v>1.7923148148148149</v>
       </c>
-      <c r="H89" s="3">
+      <c r="H89" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4638,10 +4639,10 @@
       <c r="F90" t="s">
         <v>8</v>
       </c>
-      <c r="G90" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H90" s="3">
+      <c r="G90" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H90" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4661,10 +4662,10 @@
       <c r="F91" t="s">
         <v>8</v>
       </c>
-      <c r="G91" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H91" s="3">
+      <c r="G91" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H91" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4684,10 +4685,10 @@
       <c r="F92" t="s">
         <v>8</v>
       </c>
-      <c r="G92" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H92" s="3">
+      <c r="G92" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H92" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4707,10 +4708,10 @@
       <c r="F93" t="s">
         <v>507</v>
       </c>
-      <c r="G93" s="3">
+      <c r="G93" s="5">
         <v>1.7506481481481482</v>
       </c>
-      <c r="H93" s="3">
+      <c r="H93" s="5">
         <v>1.2506481481481482</v>
       </c>
     </row>
@@ -4730,16 +4731,16 @@
       <c r="F94" t="s">
         <v>8</v>
       </c>
-      <c r="G94" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H94" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I94" s="5">
+      <c r="G94" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H94" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I94" s="4">
         <v>45719</v>
       </c>
-      <c r="J94" s="5">
+      <c r="J94" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -4759,10 +4760,10 @@
       <c r="F95" t="s">
         <v>8</v>
       </c>
-      <c r="G95" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H95" s="3">
+      <c r="G95" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H95" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4782,10 +4783,10 @@
       <c r="F96" t="s">
         <v>8</v>
       </c>
-      <c r="G96" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H96" s="3">
+      <c r="G96" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H96" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4805,10 +4806,10 @@
       <c r="F97" t="s">
         <v>8</v>
       </c>
-      <c r="G97" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H97" s="3">
+      <c r="G97" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H97" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4828,10 +4829,10 @@
       <c r="F98" t="s">
         <v>8</v>
       </c>
-      <c r="G98" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H98" s="3">
+      <c r="G98" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H98" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4851,10 +4852,10 @@
       <c r="F99" t="s">
         <v>8</v>
       </c>
-      <c r="G99" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H99" s="3">
+      <c r="G99" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H99" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4874,10 +4875,10 @@
       <c r="F100" t="s">
         <v>8</v>
       </c>
-      <c r="G100" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H100" s="3">
+      <c r="G100" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H100" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4897,10 +4898,10 @@
       <c r="F101" t="s">
         <v>8</v>
       </c>
-      <c r="G101" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H101" s="3">
+      <c r="G101" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H101" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4920,10 +4921,10 @@
       <c r="F102" t="s">
         <v>504</v>
       </c>
-      <c r="G102" s="3">
+      <c r="G102" s="5">
         <v>1.7923148148148149</v>
       </c>
-      <c r="H102" s="3">
+      <c r="H102" s="5">
         <v>1.2923148148148149</v>
       </c>
     </row>
@@ -4943,10 +4944,10 @@
       <c r="F103" t="s">
         <v>8</v>
       </c>
-      <c r="G103" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H103" s="3">
+      <c r="G103" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H103" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4966,10 +4967,10 @@
       <c r="F104" t="s">
         <v>8</v>
       </c>
-      <c r="G104" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H104" s="3">
+      <c r="G104" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H104" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -4989,10 +4990,10 @@
       <c r="F105" t="s">
         <v>8</v>
       </c>
-      <c r="G105" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H105" s="3">
+      <c r="G105" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H105" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5012,10 +5013,10 @@
       <c r="F106" t="s">
         <v>26</v>
       </c>
-      <c r="G106" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H106" s="3">
+      <c r="G106" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H106" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -5035,10 +5036,10 @@
       <c r="F107" t="s">
         <v>8</v>
       </c>
-      <c r="G107" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H107" s="3">
+      <c r="G107" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H107" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5058,10 +5059,10 @@
       <c r="F108" t="s">
         <v>8</v>
       </c>
-      <c r="G108" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H108" s="3">
+      <c r="G108" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H108" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5081,10 +5082,10 @@
       <c r="F109" t="s">
         <v>8</v>
       </c>
-      <c r="G109" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H109" s="3">
+      <c r="G109" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H109" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5104,16 +5105,16 @@
       <c r="F110" t="s">
         <v>8</v>
       </c>
-      <c r="G110" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H110" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I110" s="5">
+      <c r="G110" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H110" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I110" s="4">
         <v>45719</v>
       </c>
-      <c r="J110" s="5">
+      <c r="J110" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -5133,10 +5134,10 @@
       <c r="F111" t="s">
         <v>8</v>
       </c>
-      <c r="G111" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H111" s="3">
+      <c r="G111" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H111" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5156,10 +5157,10 @@
       <c r="F112" t="s">
         <v>8</v>
       </c>
-      <c r="G112" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H112" s="3">
+      <c r="G112" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H112" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5179,10 +5180,10 @@
       <c r="F113" t="s">
         <v>8</v>
       </c>
-      <c r="G113" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H113" s="3">
+      <c r="G113" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H113" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5202,10 +5203,10 @@
       <c r="F114" t="s">
         <v>8</v>
       </c>
-      <c r="G114" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H114" s="3">
+      <c r="G114" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H114" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5225,10 +5226,10 @@
       <c r="F115" t="s">
         <v>8</v>
       </c>
-      <c r="G115" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H115" s="3">
+      <c r="G115" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H115" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5248,10 +5249,10 @@
       <c r="F116" t="s">
         <v>8</v>
       </c>
-      <c r="G116" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H116" s="3">
+      <c r="G116" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H116" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5271,10 +5272,10 @@
       <c r="F117" t="s">
         <v>185</v>
       </c>
-      <c r="G117" s="3">
+      <c r="G117" s="5">
         <v>1.4589814814814814</v>
       </c>
-      <c r="H117" s="3">
+      <c r="H117" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5294,10 +5295,10 @@
       <c r="F118" t="s">
         <v>26</v>
       </c>
-      <c r="G118" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H118" s="3">
+      <c r="G118" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H118" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -5317,10 +5318,10 @@
       <c r="F119" t="s">
         <v>8</v>
       </c>
-      <c r="G119" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H119" s="3">
+      <c r="G119" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H119" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5340,10 +5341,10 @@
       <c r="F120" t="s">
         <v>8</v>
       </c>
-      <c r="G120" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H120" s="3">
+      <c r="G120" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H120" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5363,10 +5364,10 @@
       <c r="F121" t="s">
         <v>8</v>
       </c>
-      <c r="G121" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H121" s="3">
+      <c r="G121" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H121" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5386,10 +5387,10 @@
       <c r="F122" t="s">
         <v>8</v>
       </c>
-      <c r="G122" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H122" s="3">
+      <c r="G122" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H122" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5409,10 +5410,10 @@
       <c r="F123" t="s">
         <v>8</v>
       </c>
-      <c r="G123" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H123" s="3">
+      <c r="G123" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H123" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5432,10 +5433,10 @@
       <c r="F124" t="s">
         <v>8</v>
       </c>
-      <c r="G124" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H124" s="3">
+      <c r="G124" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H124" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5455,10 +5456,10 @@
       <c r="F125" t="s">
         <v>8</v>
       </c>
-      <c r="G125" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H125" s="3">
+      <c r="G125" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H125" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5478,10 +5479,10 @@
       <c r="F126" t="s">
         <v>8</v>
       </c>
-      <c r="G126" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H126" s="3">
+      <c r="G126" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H126" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5501,10 +5502,10 @@
       <c r="F127" t="s">
         <v>8</v>
       </c>
-      <c r="G127" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H127" s="3">
+      <c r="G127" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H127" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5524,10 +5525,10 @@
       <c r="F128" t="s">
         <v>8</v>
       </c>
-      <c r="G128" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H128" s="3">
+      <c r="G128" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H128" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5547,10 +5548,10 @@
       <c r="F129" t="s">
         <v>8</v>
       </c>
-      <c r="G129" s="3">
+      <c r="G129" s="5">
         <v>1.4589814814814814</v>
       </c>
-      <c r="H129" s="3">
+      <c r="H129" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5570,10 +5571,10 @@
       <c r="F130" t="s">
         <v>8</v>
       </c>
-      <c r="G130" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H130" s="3">
+      <c r="G130" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H130" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5593,10 +5594,10 @@
       <c r="F131" t="s">
         <v>8</v>
       </c>
-      <c r="G131" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H131" s="3">
+      <c r="G131" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H131" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5616,10 +5617,10 @@
       <c r="F132" t="s">
         <v>8</v>
       </c>
-      <c r="G132" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H132" s="3">
+      <c r="G132" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H132" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5639,10 +5640,10 @@
       <c r="F133" t="s">
         <v>8</v>
       </c>
-      <c r="G133" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H133" s="3">
+      <c r="G133" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H133" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5662,10 +5663,10 @@
       <c r="F134" t="s">
         <v>8</v>
       </c>
-      <c r="G134" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H134" s="3">
+      <c r="G134" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H134" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5685,10 +5686,10 @@
       <c r="F135" t="s">
         <v>8</v>
       </c>
-      <c r="G135" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H135" s="3">
+      <c r="G135" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H135" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5708,10 +5709,10 @@
       <c r="F136" t="s">
         <v>8</v>
       </c>
-      <c r="G136" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H136" s="3">
+      <c r="G136" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H136" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5731,10 +5732,10 @@
       <c r="F137" t="s">
         <v>8</v>
       </c>
-      <c r="G137" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H137" s="3">
+      <c r="G137" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H137" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5754,10 +5755,10 @@
       <c r="F138" t="s">
         <v>8</v>
       </c>
-      <c r="G138" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H138" s="3">
+      <c r="G138" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H138" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5777,10 +5778,10 @@
       <c r="F139" t="s">
         <v>8</v>
       </c>
-      <c r="G139" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H139" s="3">
+      <c r="G139" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H139" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5800,10 +5801,10 @@
       <c r="F140" t="s">
         <v>537</v>
       </c>
-      <c r="G140" s="3">
+      <c r="G140" s="5">
         <v>1.2923148148148149</v>
       </c>
-      <c r="H140" s="3">
+      <c r="H140" s="5">
         <v>1.7923148148148149</v>
       </c>
     </row>
@@ -5823,10 +5824,10 @@
       <c r="F141" t="s">
         <v>8</v>
       </c>
-      <c r="G141" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H141" s="3">
+      <c r="G141" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H141" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5846,10 +5847,10 @@
       <c r="F142" t="s">
         <v>8</v>
       </c>
-      <c r="G142" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H142" s="3">
+      <c r="G142" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H142" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5869,10 +5870,10 @@
       <c r="F143" t="s">
         <v>8</v>
       </c>
-      <c r="G143" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H143" s="3">
+      <c r="G143" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H143" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5892,10 +5893,10 @@
       <c r="F144" t="s">
         <v>8</v>
       </c>
-      <c r="G144" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H144" s="3">
+      <c r="G144" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H144" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5915,10 +5916,10 @@
       <c r="F145" t="s">
         <v>8</v>
       </c>
-      <c r="G145" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H145" s="3">
+      <c r="G145" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H145" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5938,10 +5939,10 @@
       <c r="F146" t="s">
         <v>8</v>
       </c>
-      <c r="G146" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H146" s="3">
+      <c r="G146" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H146" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5961,10 +5962,10 @@
       <c r="F147" t="s">
         <v>8</v>
       </c>
-      <c r="G147" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H147" s="3">
+      <c r="G147" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H147" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -5984,10 +5985,10 @@
       <c r="F148" t="s">
         <v>8</v>
       </c>
-      <c r="G148" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H148" s="3">
+      <c r="G148" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H148" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6007,10 +6008,10 @@
       <c r="F149" t="s">
         <v>8</v>
       </c>
-      <c r="G149" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H149" s="3">
+      <c r="G149" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H149" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6030,10 +6031,10 @@
       <c r="F150" t="s">
         <v>8</v>
       </c>
-      <c r="G150" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H150" s="3">
+      <c r="G150" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H150" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6053,10 +6054,10 @@
       <c r="F151" t="s">
         <v>8</v>
       </c>
-      <c r="G151" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H151" s="3">
+      <c r="G151" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H151" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6076,10 +6077,10 @@
       <c r="F152" t="s">
         <v>8</v>
       </c>
-      <c r="G152" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H152" s="3">
+      <c r="G152" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H152" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6099,10 +6100,10 @@
       <c r="F153" t="s">
         <v>8</v>
       </c>
-      <c r="G153" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H153" s="3">
+      <c r="G153" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H153" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6122,10 +6123,10 @@
       <c r="F154" t="s">
         <v>8</v>
       </c>
-      <c r="G154" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H154" s="3">
+      <c r="G154" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H154" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6145,10 +6146,10 @@
       <c r="F155" t="s">
         <v>8</v>
       </c>
-      <c r="G155" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H155" s="3">
+      <c r="G155" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H155" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6168,10 +6169,10 @@
       <c r="F156" t="s">
         <v>8</v>
       </c>
-      <c r="G156" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H156" s="3">
+      <c r="G156" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H156" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6191,10 +6192,10 @@
       <c r="F157" t="s">
         <v>8</v>
       </c>
-      <c r="G157" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H157" s="3">
+      <c r="G157" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H157" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6214,10 +6215,10 @@
       <c r="F158" t="s">
         <v>8</v>
       </c>
-      <c r="G158" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H158" s="3">
+      <c r="G158" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H158" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6237,10 +6238,10 @@
       <c r="F159" t="s">
         <v>8</v>
       </c>
-      <c r="G159" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H159" s="3">
+      <c r="G159" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H159" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6260,10 +6261,10 @@
       <c r="F160" t="s">
         <v>8</v>
       </c>
-      <c r="G160" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H160" s="3">
+      <c r="G160" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H160" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6283,10 +6284,10 @@
       <c r="F161" t="s">
         <v>8</v>
       </c>
-      <c r="G161" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H161" s="3">
+      <c r="G161" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H161" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6306,10 +6307,10 @@
       <c r="F162" t="s">
         <v>8</v>
       </c>
-      <c r="G162" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H162" s="3">
+      <c r="G162" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H162" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6329,10 +6330,10 @@
       <c r="F163" t="s">
         <v>8</v>
       </c>
-      <c r="G163" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H163" s="3">
+      <c r="G163" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H163" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6352,16 +6353,16 @@
       <c r="F164" t="s">
         <v>8</v>
       </c>
-      <c r="G164" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H164" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I164" s="5">
+      <c r="G164" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H164" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I164" s="4">
         <v>45728</v>
       </c>
-      <c r="J164" s="5">
+      <c r="J164" s="4">
         <v>45737</v>
       </c>
     </row>
@@ -6381,10 +6382,10 @@
       <c r="F165" t="s">
         <v>8</v>
       </c>
-      <c r="G165" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H165" s="3">
+      <c r="G165" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H165" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6404,10 +6405,10 @@
       <c r="F166" t="s">
         <v>8</v>
       </c>
-      <c r="G166" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H166" s="3">
+      <c r="G166" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H166" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6427,10 +6428,10 @@
       <c r="F167" t="s">
         <v>8</v>
       </c>
-      <c r="G167" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H167" s="3">
+      <c r="G167" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H167" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6450,10 +6451,10 @@
       <c r="F168" t="s">
         <v>8</v>
       </c>
-      <c r="G168" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H168" s="3">
+      <c r="G168" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H168" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6473,10 +6474,10 @@
       <c r="F169" t="s">
         <v>8</v>
       </c>
-      <c r="G169" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H169" s="3">
+      <c r="G169" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H169" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6496,10 +6497,10 @@
       <c r="F170" t="s">
         <v>8</v>
       </c>
-      <c r="G170" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H170" s="3">
+      <c r="G170" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H170" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6519,10 +6520,10 @@
       <c r="F171" t="s">
         <v>8</v>
       </c>
-      <c r="G171" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H171" s="3">
+      <c r="G171" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H171" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6542,10 +6543,10 @@
       <c r="F172" t="s">
         <v>8</v>
       </c>
-      <c r="G172" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H172" s="3">
+      <c r="G172" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H172" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6565,10 +6566,10 @@
       <c r="F173" t="s">
         <v>8</v>
       </c>
-      <c r="G173" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H173" s="3">
+      <c r="G173" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H173" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6588,10 +6589,10 @@
       <c r="F174" t="s">
         <v>8</v>
       </c>
-      <c r="G174" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H174" s="3">
+      <c r="G174" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H174" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6611,10 +6612,10 @@
       <c r="F175" t="s">
         <v>8</v>
       </c>
-      <c r="G175" s="3">
+      <c r="G175" s="5">
         <v>1.4589814814814814</v>
       </c>
-      <c r="H175" s="3">
+      <c r="H175" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6634,10 +6635,10 @@
       <c r="F176" t="s">
         <v>8</v>
       </c>
-      <c r="G176" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H176" s="3">
+      <c r="G176" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H176" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6657,10 +6658,10 @@
       <c r="F177" t="s">
         <v>26</v>
       </c>
-      <c r="G177" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H177" s="3">
+      <c r="G177" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H177" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -6680,10 +6681,10 @@
       <c r="F178" t="s">
         <v>8</v>
       </c>
-      <c r="G178" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H178" s="3">
+      <c r="G178" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H178" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6703,10 +6704,10 @@
       <c r="F179" t="s">
         <v>8</v>
       </c>
-      <c r="G179" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H179" s="3">
+      <c r="G179" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H179" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6726,10 +6727,10 @@
       <c r="F180" t="s">
         <v>8</v>
       </c>
-      <c r="G180" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H180" s="3">
+      <c r="G180" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H180" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6749,10 +6750,10 @@
       <c r="F181" t="s">
         <v>8</v>
       </c>
-      <c r="G181" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H181" s="3">
+      <c r="G181" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H181" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6772,10 +6773,10 @@
       <c r="F182" t="s">
         <v>8</v>
       </c>
-      <c r="G182" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H182" s="3">
+      <c r="G182" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H182" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6795,10 +6796,10 @@
       <c r="F183" t="s">
         <v>8</v>
       </c>
-      <c r="G183" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H183" s="3">
+      <c r="G183" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H183" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6818,10 +6819,10 @@
       <c r="F184" t="s">
         <v>8</v>
       </c>
-      <c r="G184" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H184" s="3">
+      <c r="G184" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H184" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6841,16 +6842,16 @@
       <c r="F185" t="s">
         <v>8</v>
       </c>
-      <c r="G185" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H185" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I185" s="5">
+      <c r="G185" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H185" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I185" s="4">
         <v>45719</v>
       </c>
-      <c r="J185" s="5">
+      <c r="J185" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -6870,10 +6871,10 @@
       <c r="F186" t="s">
         <v>8</v>
       </c>
-      <c r="G186" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H186" s="3">
+      <c r="G186" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H186" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6893,10 +6894,10 @@
       <c r="F187" t="s">
         <v>8</v>
       </c>
-      <c r="G187" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H187" s="3">
+      <c r="G187" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H187" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6916,16 +6917,16 @@
       <c r="F188" t="s">
         <v>8</v>
       </c>
-      <c r="G188" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H188" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I188" s="5">
+      <c r="G188" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H188" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I188" s="4">
         <v>45719</v>
       </c>
-      <c r="J188" s="5">
+      <c r="J188" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -6945,10 +6946,10 @@
       <c r="F189" t="s">
         <v>8</v>
       </c>
-      <c r="G189" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H189" s="3">
+      <c r="G189" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H189" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -6968,16 +6969,16 @@
       <c r="F190" t="s">
         <v>26</v>
       </c>
-      <c r="G190" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H190" s="3">
+      <c r="G190" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H190" s="5">
         <v>1.5839814814814814</v>
       </c>
-      <c r="I190" s="5">
+      <c r="I190" s="4">
         <v>45719</v>
       </c>
-      <c r="J190" s="5">
+      <c r="J190" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -6997,10 +6998,10 @@
       <c r="F191" t="s">
         <v>26</v>
       </c>
-      <c r="G191" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H191" s="3">
+      <c r="G191" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H191" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -7020,10 +7021,10 @@
       <c r="F192" t="s">
         <v>8</v>
       </c>
-      <c r="G192" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H192" s="3">
+      <c r="G192" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H192" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7043,10 +7044,10 @@
       <c r="F193" t="s">
         <v>8</v>
       </c>
-      <c r="G193" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H193" s="3">
+      <c r="G193" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H193" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7066,10 +7067,10 @@
       <c r="F194" t="s">
         <v>8</v>
       </c>
-      <c r="G194" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H194" s="3">
+      <c r="G194" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H194" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7089,10 +7090,10 @@
       <c r="F195" t="s">
         <v>8</v>
       </c>
-      <c r="G195" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H195" s="3">
+      <c r="G195" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H195" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7112,10 +7113,10 @@
       <c r="F196" t="s">
         <v>8</v>
       </c>
-      <c r="G196" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H196" s="3">
+      <c r="G196" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H196" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7135,10 +7136,10 @@
       <c r="F197" t="s">
         <v>8</v>
       </c>
-      <c r="G197" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H197" s="3">
+      <c r="G197" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H197" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7158,10 +7159,10 @@
       <c r="F198" t="s">
         <v>8</v>
       </c>
-      <c r="G198" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H198" s="3">
+      <c r="G198" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H198" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7181,10 +7182,10 @@
       <c r="F199" t="s">
         <v>8</v>
       </c>
-      <c r="G199" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H199" s="3">
+      <c r="G199" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H199" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7204,10 +7205,10 @@
       <c r="F200" t="s">
         <v>8</v>
       </c>
-      <c r="G200" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H200" s="3">
+      <c r="G200" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H200" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7227,10 +7228,10 @@
       <c r="F201" t="s">
         <v>8</v>
       </c>
-      <c r="G201" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H201" s="3">
+      <c r="G201" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H201" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7250,10 +7251,10 @@
       <c r="F202" t="s">
         <v>8</v>
       </c>
-      <c r="G202" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H202" s="3">
+      <c r="G202" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H202" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7273,10 +7274,10 @@
       <c r="F203" t="s">
         <v>8</v>
       </c>
-      <c r="G203" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H203" s="3">
+      <c r="G203" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H203" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7296,10 +7297,10 @@
       <c r="F204" t="s">
         <v>8</v>
       </c>
-      <c r="G204" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H204" s="3">
+      <c r="G204" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H204" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7319,10 +7320,10 @@
       <c r="F205" t="s">
         <v>26</v>
       </c>
-      <c r="G205" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H205" s="3">
+      <c r="G205" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H205" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -7342,10 +7343,10 @@
       <c r="F206" t="s">
         <v>8</v>
       </c>
-      <c r="G206" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H206" s="3">
+      <c r="G206" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H206" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7365,10 +7366,10 @@
       <c r="F207" t="s">
         <v>8</v>
       </c>
-      <c r="G207" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H207" s="3">
+      <c r="G207" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H207" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7388,10 +7389,10 @@
       <c r="F208" t="s">
         <v>8</v>
       </c>
-      <c r="G208" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H208" s="3">
+      <c r="G208" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H208" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7411,10 +7412,10 @@
       <c r="F209" t="s">
         <v>8</v>
       </c>
-      <c r="G209" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H209" s="3">
+      <c r="G209" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H209" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7434,10 +7435,10 @@
       <c r="F210" t="s">
         <v>8</v>
       </c>
-      <c r="G210" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H210" s="3">
+      <c r="G210" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H210" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7457,10 +7458,10 @@
       <c r="F211" t="s">
         <v>8</v>
       </c>
-      <c r="G211" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H211" s="3">
+      <c r="G211" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H211" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7480,10 +7481,10 @@
       <c r="F212" t="s">
         <v>8</v>
       </c>
-      <c r="G212" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H212" s="3">
+      <c r="G212" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H212" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7503,10 +7504,10 @@
       <c r="F213" t="s">
         <v>8</v>
       </c>
-      <c r="G213" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H213" s="3">
+      <c r="G213" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H213" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7526,10 +7527,10 @@
       <c r="F214" t="s">
         <v>26</v>
       </c>
-      <c r="G214" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H214" s="3">
+      <c r="G214" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H214" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -7549,10 +7550,10 @@
       <c r="F215" t="s">
         <v>8</v>
       </c>
-      <c r="G215" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H215" s="3">
+      <c r="G215" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H215" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7572,10 +7573,10 @@
       <c r="F216" t="s">
         <v>8</v>
       </c>
-      <c r="G216" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H216" s="3">
+      <c r="G216" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H216" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7595,10 +7596,10 @@
       <c r="F217" t="s">
         <v>8</v>
       </c>
-      <c r="G217" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H217" s="3">
+      <c r="G217" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H217" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7618,10 +7619,10 @@
       <c r="F218" t="s">
         <v>26</v>
       </c>
-      <c r="G218" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H218" s="3">
+      <c r="G218" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H218" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -7641,10 +7642,10 @@
       <c r="F219" t="s">
         <v>8</v>
       </c>
-      <c r="G219" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H219" s="3">
+      <c r="G219" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H219" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7664,10 +7665,10 @@
       <c r="F220" t="s">
         <v>8</v>
       </c>
-      <c r="G220" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H220" s="3">
+      <c r="G220" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H220" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7687,10 +7688,10 @@
       <c r="F221" t="s">
         <v>8</v>
       </c>
-      <c r="G221" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H221" s="3">
+      <c r="G221" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H221" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7710,10 +7711,10 @@
       <c r="F222" t="s">
         <v>8</v>
       </c>
-      <c r="G222" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H222" s="3">
+      <c r="G222" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H222" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7733,10 +7734,10 @@
       <c r="F223" t="s">
         <v>8</v>
       </c>
-      <c r="G223" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H223" s="3">
+      <c r="G223" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H223" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7756,10 +7757,10 @@
       <c r="F224" t="s">
         <v>8</v>
       </c>
-      <c r="G224" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H224" s="3">
+      <c r="G224" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H224" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7779,16 +7780,16 @@
       <c r="F225" t="s">
         <v>8</v>
       </c>
-      <c r="G225" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H225" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I225" s="5">
+      <c r="G225" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H225" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I225" s="4">
         <v>45719</v>
       </c>
-      <c r="J225" s="5">
+      <c r="J225" s="4">
         <v>45748</v>
       </c>
     </row>
@@ -7808,10 +7809,10 @@
       <c r="F226" t="s">
         <v>8</v>
       </c>
-      <c r="G226" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H226" s="3">
+      <c r="G226" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H226" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7831,10 +7832,10 @@
       <c r="F227" t="s">
         <v>8</v>
       </c>
-      <c r="G227" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H227" s="3">
+      <c r="G227" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H227" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7854,10 +7855,10 @@
       <c r="F228" t="s">
         <v>8</v>
       </c>
-      <c r="G228" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H228" s="3">
+      <c r="G228" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H228" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7877,10 +7878,10 @@
       <c r="F229" t="s">
         <v>8</v>
       </c>
-      <c r="G229" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H229" s="3">
+      <c r="G229" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H229" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7900,10 +7901,10 @@
       <c r="F230" t="s">
         <v>8</v>
       </c>
-      <c r="G230" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H230" s="3">
+      <c r="G230" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H230" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7923,10 +7924,10 @@
       <c r="F231" t="s">
         <v>8</v>
       </c>
-      <c r="G231" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H231" s="3">
+      <c r="G231" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H231" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7946,10 +7947,10 @@
       <c r="F232" t="s">
         <v>8</v>
       </c>
-      <c r="G232" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H232" s="3">
+      <c r="G232" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H232" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -7969,10 +7970,10 @@
       <c r="F233" t="s">
         <v>26</v>
       </c>
-      <c r="G233" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H233" s="3">
+      <c r="G233" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H233" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -7992,10 +7993,10 @@
       <c r="F234" t="s">
         <v>8</v>
       </c>
-      <c r="G234" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H234" s="3">
+      <c r="G234" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H234" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8015,10 +8016,10 @@
       <c r="F235" t="s">
         <v>8</v>
       </c>
-      <c r="G235" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H235" s="3">
+      <c r="G235" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H235" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8038,10 +8039,10 @@
       <c r="F236" t="s">
         <v>8</v>
       </c>
-      <c r="G236" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H236" s="3">
+      <c r="G236" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H236" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8061,10 +8062,10 @@
       <c r="F237" t="s">
         <v>8</v>
       </c>
-      <c r="G237" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H237" s="3">
+      <c r="G237" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H237" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8084,10 +8085,10 @@
       <c r="F238" t="s">
         <v>8</v>
       </c>
-      <c r="G238" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H238" s="3">
+      <c r="G238" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H238" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8107,10 +8108,10 @@
       <c r="F239" t="s">
         <v>8</v>
       </c>
-      <c r="G239" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H239" s="3">
+      <c r="G239" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H239" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8130,10 +8131,10 @@
       <c r="F240" t="s">
         <v>8</v>
       </c>
-      <c r="G240" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H240" s="3">
+      <c r="G240" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H240" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8153,16 +8154,16 @@
       <c r="F241" t="s">
         <v>8</v>
       </c>
-      <c r="G241" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H241" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I241" s="5">
+      <c r="G241" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H241" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I241" s="4">
         <v>45722</v>
       </c>
-      <c r="J241" s="5">
+      <c r="J241" s="4">
         <v>45731</v>
       </c>
     </row>
@@ -8182,10 +8183,10 @@
       <c r="F242" t="s">
         <v>8</v>
       </c>
-      <c r="G242" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H242" s="3">
+      <c r="G242" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H242" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8205,10 +8206,10 @@
       <c r="F243" t="s">
         <v>8</v>
       </c>
-      <c r="G243" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H243" s="3">
+      <c r="G243" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H243" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8228,10 +8229,10 @@
       <c r="F244" t="s">
         <v>8</v>
       </c>
-      <c r="G244" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H244" s="3">
+      <c r="G244" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H244" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8251,10 +8252,10 @@
       <c r="F245" t="s">
         <v>8</v>
       </c>
-      <c r="G245" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H245" s="3">
+      <c r="G245" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H245" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8274,10 +8275,10 @@
       <c r="F246" t="s">
         <v>8</v>
       </c>
-      <c r="G246" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H246" s="3">
+      <c r="G246" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H246" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8297,10 +8298,10 @@
       <c r="F247" t="s">
         <v>8</v>
       </c>
-      <c r="G247" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H247" s="3">
+      <c r="G247" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H247" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8320,10 +8321,10 @@
       <c r="F248" t="s">
         <v>26</v>
       </c>
-      <c r="G248" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H248" s="3">
+      <c r="G248" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H248" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -8343,10 +8344,10 @@
       <c r="F249" t="s">
         <v>8</v>
       </c>
-      <c r="G249" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H249" s="3">
+      <c r="G249" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H249" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8366,16 +8367,16 @@
       <c r="F250" t="s">
         <v>8</v>
       </c>
-      <c r="G250" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H250" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I250" s="5">
+      <c r="G250" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H250" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I250" s="4">
         <v>45733</v>
       </c>
-      <c r="J250" s="5">
+      <c r="J250" s="4">
         <v>45747</v>
       </c>
     </row>
@@ -8392,10 +8393,10 @@
       <c r="F251" t="s">
         <v>8</v>
       </c>
-      <c r="G251" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H251" s="3">
+      <c r="G251" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H251" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8415,10 +8416,10 @@
       <c r="F252" t="s">
         <v>8</v>
       </c>
-      <c r="G252" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H252" s="3">
+      <c r="G252" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H252" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8438,10 +8439,10 @@
       <c r="F253" t="s">
         <v>8</v>
       </c>
-      <c r="G253" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H253" s="3">
+      <c r="G253" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H253" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8461,10 +8462,10 @@
       <c r="F254" t="s">
         <v>8</v>
       </c>
-      <c r="G254" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H254" s="3">
+      <c r="G254" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H254" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8484,10 +8485,10 @@
       <c r="F255" t="s">
         <v>8</v>
       </c>
-      <c r="G255" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H255" s="3">
+      <c r="G255" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H255" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8507,10 +8508,10 @@
       <c r="F256" t="s">
         <v>8</v>
       </c>
-      <c r="G256" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H256" s="3">
+      <c r="G256" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H256" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8530,10 +8531,10 @@
       <c r="F257" t="s">
         <v>8</v>
       </c>
-      <c r="G257" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H257" s="3">
+      <c r="G257" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H257" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8553,10 +8554,10 @@
       <c r="F258" t="s">
         <v>8</v>
       </c>
-      <c r="G258" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H258" s="3">
+      <c r="G258" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H258" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8576,10 +8577,10 @@
       <c r="F259" t="s">
         <v>185</v>
       </c>
-      <c r="G259" s="3">
+      <c r="G259" s="5">
         <v>1.4589814814814814</v>
       </c>
-      <c r="H259" s="3">
+      <c r="H259" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8599,10 +8600,10 @@
       <c r="F260" t="s">
         <v>8</v>
       </c>
-      <c r="G260" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H260" s="3">
+      <c r="G260" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H260" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8622,10 +8623,10 @@
       <c r="F261" t="s">
         <v>8</v>
       </c>
-      <c r="G261" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H261" s="3">
+      <c r="G261" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H261" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8645,10 +8646,10 @@
       <c r="F262" t="s">
         <v>8</v>
       </c>
-      <c r="G262" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H262" s="3">
+      <c r="G262" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H262" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8668,10 +8669,10 @@
       <c r="F263" t="s">
         <v>8</v>
       </c>
-      <c r="G263" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H263" s="3">
+      <c r="G263" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H263" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8691,10 +8692,10 @@
       <c r="F264" t="s">
         <v>8</v>
       </c>
-      <c r="G264" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H264" s="3">
+      <c r="G264" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H264" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8714,16 +8715,16 @@
       <c r="F265" t="s">
         <v>8</v>
       </c>
-      <c r="G265" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H265" s="3">
-        <v>1.7089814814814814</v>
-      </c>
-      <c r="I265" s="5">
+      <c r="G265" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H265" s="5">
+        <v>1.7089814814814814</v>
+      </c>
+      <c r="I265" s="4">
         <v>45726</v>
       </c>
-      <c r="J265" s="5">
+      <c r="J265" s="4">
         <v>45730</v>
       </c>
     </row>
@@ -8743,10 +8744,10 @@
       <c r="F266" t="s">
         <v>8</v>
       </c>
-      <c r="G266" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H266" s="3">
+      <c r="G266" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H266" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8766,10 +8767,10 @@
       <c r="F267" t="s">
         <v>8</v>
       </c>
-      <c r="G267" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H267" s="3">
+      <c r="G267" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H267" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8789,10 +8790,10 @@
       <c r="F268" t="s">
         <v>8</v>
       </c>
-      <c r="G268" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H268" s="3">
+      <c r="G268" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H268" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8812,10 +8813,10 @@
       <c r="F269" t="s">
         <v>8</v>
       </c>
-      <c r="G269" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H269" s="3">
+      <c r="G269" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H269" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8835,10 +8836,10 @@
       <c r="F270" t="s">
         <v>8</v>
       </c>
-      <c r="G270" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H270" s="3">
+      <c r="G270" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H270" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8858,10 +8859,10 @@
       <c r="F271" t="s">
         <v>8</v>
       </c>
-      <c r="G271" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H271" s="3">
+      <c r="G271" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H271" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8881,10 +8882,10 @@
       <c r="F272" t="s">
         <v>8</v>
       </c>
-      <c r="G272" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H272" s="3">
+      <c r="G272" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H272" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8904,10 +8905,10 @@
       <c r="F273" t="s">
         <v>26</v>
       </c>
-      <c r="G273" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H273" s="3">
+      <c r="G273" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H273" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -8927,10 +8928,10 @@
       <c r="F274" t="s">
         <v>8</v>
       </c>
-      <c r="G274" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H274" s="3">
+      <c r="G274" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H274" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8950,10 +8951,10 @@
       <c r="F275" t="s">
         <v>8</v>
       </c>
-      <c r="G275" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H275" s="3">
+      <c r="G275" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H275" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8973,10 +8974,10 @@
       <c r="F276" t="s">
         <v>8</v>
       </c>
-      <c r="G276" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H276" s="3">
+      <c r="G276" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H276" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -8996,10 +8997,10 @@
       <c r="F277" t="s">
         <v>8</v>
       </c>
-      <c r="G277" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H277" s="3">
+      <c r="G277" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H277" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9019,10 +9020,10 @@
       <c r="F278" t="s">
         <v>8</v>
       </c>
-      <c r="G278" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H278" s="3">
+      <c r="G278" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H278" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9042,10 +9043,10 @@
       <c r="F279" t="s">
         <v>8</v>
       </c>
-      <c r="G279" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H279" s="3">
+      <c r="G279" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H279" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9065,10 +9066,10 @@
       <c r="F280" t="s">
         <v>8</v>
       </c>
-      <c r="G280" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H280" s="3">
+      <c r="G280" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H280" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9088,10 +9089,10 @@
       <c r="F281" t="s">
         <v>8</v>
       </c>
-      <c r="G281" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H281" s="3">
+      <c r="G281" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H281" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9111,10 +9112,10 @@
       <c r="F282" t="s">
         <v>8</v>
       </c>
-      <c r="G282" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H282" s="3">
+      <c r="G282" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H282" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9134,10 +9135,10 @@
       <c r="F283" t="s">
         <v>26</v>
       </c>
-      <c r="G283" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H283" s="3">
+      <c r="G283" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H283" s="5">
         <v>1.5839814814814814</v>
       </c>
     </row>
@@ -9157,10 +9158,10 @@
       <c r="F284" t="s">
         <v>8</v>
       </c>
-      <c r="G284" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H284" s="3">
+      <c r="G284" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H284" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9180,10 +9181,10 @@
       <c r="F285" t="s">
         <v>8</v>
       </c>
-      <c r="G285" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H285" s="3">
+      <c r="G285" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H285" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9203,10 +9204,10 @@
       <c r="F286" t="s">
         <v>8</v>
       </c>
-      <c r="G286" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H286" s="3">
+      <c r="G286" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H286" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9226,10 +9227,10 @@
       <c r="F287" t="s">
         <v>8</v>
       </c>
-      <c r="G287" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H287" s="3">
+      <c r="G287" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H287" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9249,10 +9250,10 @@
       <c r="F288" t="s">
         <v>8</v>
       </c>
-      <c r="G288" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H288" s="3">
+      <c r="G288" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H288" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9272,10 +9273,10 @@
       <c r="F289" t="s">
         <v>8</v>
       </c>
-      <c r="G289" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H289" s="3">
+      <c r="G289" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H289" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>
@@ -9295,10 +9296,10 @@
       <c r="F290" t="s">
         <v>8</v>
       </c>
-      <c r="G290" s="3">
-        <v>1.3339814814814814</v>
-      </c>
-      <c r="H290" s="3">
+      <c r="G290" s="5">
+        <v>1.3339814814814814</v>
+      </c>
+      <c r="H290" s="5">
         <v>1.7089814814814814</v>
       </c>
     </row>

</xml_diff>